<commit_message>
Get PartNames in Rack
</commit_message>
<xml_diff>
--- a/TspuWebPortal/Development/unsafe_uploads/DC1_Rack_9.xlsx
+++ b/TspuWebPortal/Development/unsafe_uploads/DC1_Rack_9.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
-    <sheet name="Rack 7" sheetId="3" r:id="rId1"/>
+    <sheet name="Rack 9" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1286,7 +1286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>

</xml_diff>